<commit_message>
Finished monthly average AQHI dataset
</commit_message>
<xml_diff>
--- a/csv_to_excel/2020-2022_AQHI_monthly_average.xlsx
+++ b/csv_to_excel/2020-2022_AQHI_monthly_average.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sasoffice365-my.sharepoint.com/personal/wilson_leung_sas_com/Documents/Desktop/seem_data_proj/csv_to_excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AEA73896-9C4B-4A87-9A1B-3F0643BAB603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="8_{AEA73896-9C4B-4A87-9A1B-3F0643BAB603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{96FA75BC-591A-4867-88E6-9FF81E0D043E}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{DAA009C8-3F5E-47F6-BF7F-EE3B6C327CD5}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -575,8 +574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52092026-4B43-428D-8FDA-ECCFD387E24C}">
   <dimension ref="A1:Q37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24:Q24"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1957,55 +1956,583 @@
       <c r="A27" t="s">
         <v>41</v>
       </c>
+      <c r="B27">
+        <v>3.1800595238095242</v>
+      </c>
+      <c r="C27">
+        <v>2.9940476190476191</v>
+      </c>
+      <c r="D27">
+        <v>3.1934523809523809</v>
+      </c>
+      <c r="E27">
+        <v>3.0610119047619051</v>
+      </c>
+      <c r="F27">
+        <v>3.041666666666667</v>
+      </c>
+      <c r="G27">
+        <v>2.8258928571428572</v>
+      </c>
+      <c r="H27">
+        <v>2.816964285714286</v>
+      </c>
+      <c r="I27">
+        <v>2.8973214285714279</v>
+      </c>
+      <c r="J27">
+        <v>2.796130952380953</v>
+      </c>
+      <c r="K27">
+        <v>2.8184523809523809</v>
+      </c>
+      <c r="L27">
+        <v>2.59375</v>
+      </c>
+      <c r="M27">
+        <v>2.8556547619047619</v>
+      </c>
+      <c r="N27">
+        <v>2.8214285714285721</v>
+      </c>
+      <c r="O27">
+        <v>2.8363095238095242</v>
+      </c>
+      <c r="P27">
+        <v>2.808383233532934</v>
+      </c>
+      <c r="Q27">
+        <v>3.15625</v>
+      </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>42</v>
       </c>
+      <c r="B28">
+        <v>3.860215053763441</v>
+      </c>
+      <c r="C28">
+        <v>3.471774193548387</v>
+      </c>
+      <c r="D28">
+        <v>3.84005376344086</v>
+      </c>
+      <c r="E28">
+        <v>3.763440860215054</v>
+      </c>
+      <c r="F28">
+        <v>3.635752688172043</v>
+      </c>
+      <c r="G28">
+        <v>3.450268817204301</v>
+      </c>
+      <c r="H28">
+        <v>3.307795698924731</v>
+      </c>
+      <c r="I28">
+        <v>3.588709677419355</v>
+      </c>
+      <c r="J28">
+        <v>3.19758064516129</v>
+      </c>
+      <c r="K28">
+        <v>3.400537634408602</v>
+      </c>
+      <c r="L28">
+        <v>2.9946236559139781</v>
+      </c>
+      <c r="M28">
+        <v>3.556451612903226</v>
+      </c>
+      <c r="N28">
+        <v>3.344086021505376</v>
+      </c>
+      <c r="O28">
+        <v>3.385752688172043</v>
+      </c>
+      <c r="P28">
+        <v>3.3766937669376689</v>
+      </c>
+      <c r="Q28">
+        <v>3.637096774193548</v>
+      </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>43</v>
       </c>
+      <c r="B29">
+        <v>3.6541666666666668</v>
+      </c>
+      <c r="C29">
+        <v>3.4874999999999998</v>
+      </c>
+      <c r="D29">
+        <v>3.7361111111111112</v>
+      </c>
+      <c r="E29">
+        <v>3.6694444444444438</v>
+      </c>
+      <c r="F29">
+        <v>3.6430555555555562</v>
+      </c>
+      <c r="G29">
+        <v>3.458333333333333</v>
+      </c>
+      <c r="H29">
+        <v>3.2527777777777782</v>
+      </c>
+      <c r="I29">
+        <v>3.5277777777777781</v>
+      </c>
+      <c r="J29">
+        <v>3.4361111111111109</v>
+      </c>
+      <c r="K29">
+        <v>3.4777777777777779</v>
+      </c>
+      <c r="L29">
+        <v>3.119444444444444</v>
+      </c>
+      <c r="M29">
+        <v>3.568055555555556</v>
+      </c>
+      <c r="N29">
+        <v>3.3708333333333331</v>
+      </c>
+      <c r="O29">
+        <v>3.4486111111111111</v>
+      </c>
+      <c r="P29">
+        <v>3.347826086956522</v>
+      </c>
+      <c r="Q29">
+        <v>3.5222222222222221</v>
+      </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>44</v>
       </c>
+      <c r="B30">
+        <v>3.370967741935484</v>
+      </c>
+      <c r="C30">
+        <v>3.205645161290323</v>
+      </c>
+      <c r="D30">
+        <v>3.5053763440860219</v>
+      </c>
+      <c r="E30">
+        <v>3.341397849462366</v>
+      </c>
+      <c r="F30">
+        <v>3.342741935483871</v>
+      </c>
+      <c r="G30">
+        <v>3.268817204301075</v>
+      </c>
+      <c r="H30">
+        <v>3.1411290322580649</v>
+      </c>
+      <c r="I30">
+        <v>3.259408602150538</v>
+      </c>
+      <c r="J30">
+        <v>3.091397849462366</v>
+      </c>
+      <c r="K30">
+        <v>3.143817204301075</v>
+      </c>
+      <c r="L30">
+        <v>2.758064516129032</v>
+      </c>
+      <c r="M30">
+        <v>3.225806451612903</v>
+      </c>
+      <c r="N30">
+        <v>3.143817204301075</v>
+      </c>
+      <c r="O30">
+        <v>3.205645161290323</v>
+      </c>
+      <c r="P30">
+        <v>3.1972789115646258</v>
+      </c>
+      <c r="Q30">
+        <v>3.341397849462366</v>
+      </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>45</v>
       </c>
+      <c r="B31">
+        <v>2.2124999999999999</v>
+      </c>
+      <c r="C31">
+        <v>2.1138888888888889</v>
+      </c>
+      <c r="D31">
+        <v>2.3611111111111112</v>
+      </c>
+      <c r="E31">
+        <v>2.255555555555556</v>
+      </c>
+      <c r="F31">
+        <v>2.208333333333333</v>
+      </c>
+      <c r="G31">
+        <v>2.2777777777777781</v>
+      </c>
+      <c r="H31">
+        <v>2.1833333333333331</v>
+      </c>
+      <c r="I31">
+        <v>2.0972222222222219</v>
+      </c>
+      <c r="J31">
+        <v>2.0555555555555549</v>
+      </c>
+      <c r="K31">
+        <v>2.0819444444444439</v>
+      </c>
+      <c r="L31">
+        <v>1.8638888888888889</v>
+      </c>
+      <c r="M31">
+        <v>2.072222222222222</v>
+      </c>
+      <c r="N31">
+        <v>2.0541666666666671</v>
+      </c>
+      <c r="O31">
+        <v>2.0180555555555562</v>
+      </c>
+      <c r="P31">
+        <v>1.9282639885222379</v>
+      </c>
+      <c r="Q31">
+        <v>2.3736111111111109</v>
+      </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B32">
+        <v>2.692204301075269</v>
+      </c>
+      <c r="C32">
+        <v>2.416666666666667</v>
+      </c>
+      <c r="D32">
+        <v>2.774193548387097</v>
+      </c>
+      <c r="E32">
+        <v>2.665322580645161</v>
+      </c>
+      <c r="F32">
+        <v>2.635752688172043</v>
+      </c>
+      <c r="G32">
+        <v>2.625</v>
+      </c>
+      <c r="H32">
+        <v>2.475806451612903</v>
+      </c>
+      <c r="I32">
+        <v>2.497311827956989</v>
+      </c>
+      <c r="J32">
+        <v>2.491935483870968</v>
+      </c>
+      <c r="K32">
+        <v>2.4946236559139781</v>
+      </c>
+      <c r="L32">
+        <v>2.189516129032258</v>
+      </c>
+      <c r="M32">
+        <v>2.6088709677419351</v>
+      </c>
+      <c r="N32">
+        <v>2.514784946236559</v>
+      </c>
+      <c r="O32">
+        <v>2.684139784946237</v>
+      </c>
+      <c r="P32">
+        <v>2.3799185888738128</v>
+      </c>
+      <c r="Q32">
+        <v>2.84005376344086</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B33">
+        <v>2.770161290322581</v>
+      </c>
+      <c r="C33">
+        <v>2.4516129032258061</v>
+      </c>
+      <c r="D33">
+        <v>2.870967741935484</v>
+      </c>
+      <c r="E33">
+        <v>2.5981182795698921</v>
+      </c>
+      <c r="F33">
+        <v>2.6733870967741939</v>
+      </c>
+      <c r="G33">
+        <v>2.55241935483871</v>
+      </c>
+      <c r="H33">
+        <v>2.46505376344086</v>
+      </c>
+      <c r="I33">
+        <v>2.501344086021505</v>
+      </c>
+      <c r="J33">
+        <v>2.342741935483871</v>
+      </c>
+      <c r="K33">
+        <v>2.638440860215054</v>
+      </c>
+      <c r="L33">
+        <v>2.25</v>
+      </c>
+      <c r="M33">
+        <v>2.567204301075269</v>
+      </c>
+      <c r="N33">
+        <v>2.495967741935484</v>
+      </c>
+      <c r="O33">
+        <v>2.579301075268817</v>
+      </c>
+      <c r="P33">
+        <v>2.458108108108108</v>
+      </c>
+      <c r="Q33">
+        <v>2.940860215053763</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B34">
+        <v>5.4722222222222223</v>
+      </c>
+      <c r="C34">
+        <v>4.8250000000000002</v>
+      </c>
+      <c r="D34">
+        <v>5.1833333333333336</v>
+      </c>
+      <c r="E34">
+        <v>4.8361111111111112</v>
+      </c>
+      <c r="F34">
+        <v>5.1472222222222221</v>
+      </c>
+      <c r="G34">
+        <v>4.697222222222222</v>
+      </c>
+      <c r="H34">
+        <v>4.7874999999999996</v>
+      </c>
+      <c r="I34">
+        <v>4.7263888888888888</v>
+      </c>
+      <c r="J34">
+        <v>4.7833333333333332</v>
+      </c>
+      <c r="K34">
+        <v>5.1958333333333337</v>
+      </c>
+      <c r="L34">
+        <v>4.3944444444444448</v>
+      </c>
+      <c r="M34">
+        <v>4.7680555555555557</v>
+      </c>
+      <c r="N34">
+        <v>4.7374999999999998</v>
+      </c>
+      <c r="O34">
+        <v>4.7166666666666668</v>
+      </c>
+      <c r="P34">
+        <v>4.6215083798882679</v>
+      </c>
+      <c r="Q34">
+        <v>5.0236111111111112</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B35">
+        <v>4.198924731182796</v>
+      </c>
+      <c r="C35">
+        <v>4.096774193548387</v>
+      </c>
+      <c r="D35">
+        <v>4.309139784946237</v>
+      </c>
+      <c r="E35">
+        <v>4.014784946236559</v>
+      </c>
+      <c r="F35">
+        <v>4.17741935483871</v>
+      </c>
+      <c r="G35">
+        <v>3.854838709677419</v>
+      </c>
+      <c r="H35">
+        <v>3.873655913978495</v>
+      </c>
+      <c r="I35">
+        <v>3.888440860215054</v>
+      </c>
+      <c r="J35">
+        <v>4.344086021505376</v>
+      </c>
+      <c r="K35">
+        <v>4.372311827956989</v>
+      </c>
+      <c r="L35">
+        <v>3.708333333333333</v>
+      </c>
+      <c r="M35">
+        <v>3.958333333333333</v>
+      </c>
+      <c r="N35">
+        <v>3.970430107526882</v>
+      </c>
+      <c r="O35">
+        <v>4.049731182795699</v>
+      </c>
+      <c r="P35">
+        <v>4.0197740112994351</v>
+      </c>
+      <c r="Q35">
+        <v>4.115591397849462</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B36">
+        <v>3.2875000000000001</v>
+      </c>
+      <c r="C36">
+        <v>3.286111111111111</v>
+      </c>
+      <c r="D36">
+        <v>3.5597222222222218</v>
+      </c>
+      <c r="E36">
+        <v>3.1638888888888892</v>
+      </c>
+      <c r="F36">
+        <v>3.3236111111111111</v>
+      </c>
+      <c r="G36">
+        <v>2.9152777777777779</v>
+      </c>
+      <c r="H36">
+        <v>2.9805555555555561</v>
+      </c>
+      <c r="I36">
+        <v>3.161111111111111</v>
+      </c>
+      <c r="J36">
+        <v>3.1597222222222219</v>
+      </c>
+      <c r="K36">
+        <v>3.1652777777777779</v>
+      </c>
+      <c r="L36">
+        <v>2.770833333333333</v>
+      </c>
+      <c r="M36">
+        <v>3.1069444444444438</v>
+      </c>
+      <c r="N36">
+        <v>3.05</v>
+      </c>
+      <c r="O36">
+        <v>3.0874999999999999</v>
+      </c>
+      <c r="P36">
+        <v>3.0154061624649859</v>
+      </c>
+      <c r="Q36">
+        <v>3.3944444444444439</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>51</v>
+      </c>
+      <c r="B37">
+        <v>3.342741935483871</v>
+      </c>
+      <c r="C37">
+        <v>3.381720430107527</v>
+      </c>
+      <c r="D37">
+        <v>3.512096774193548</v>
+      </c>
+      <c r="E37">
+        <v>3.192204301075269</v>
+      </c>
+      <c r="F37">
+        <v>3.30510752688172</v>
+      </c>
+      <c r="G37">
+        <v>3.111559139784946</v>
+      </c>
+      <c r="H37">
+        <v>3.036290322580645</v>
+      </c>
+      <c r="I37">
+        <v>3.158602150537634</v>
+      </c>
+      <c r="J37">
+        <v>3.543010752688172</v>
+      </c>
+      <c r="K37">
+        <v>3.452956989247312</v>
+      </c>
+      <c r="L37">
+        <v>2.834677419354839</v>
+      </c>
+      <c r="M37">
+        <v>3.03494623655914</v>
+      </c>
+      <c r="N37">
+        <v>3.057795698924731</v>
+      </c>
+      <c r="O37">
+        <v>3.125</v>
+      </c>
+      <c r="P37">
+        <v>3.008163265306123</v>
+      </c>
+      <c r="Q37">
+        <v>3.666666666666667</v>
       </c>
     </row>
   </sheetData>

</xml_diff>